<commit_message>
New results of experiments
</commit_message>
<xml_diff>
--- a/results/resultados consolidados heuristicas.xlsx
+++ b/results/resultados consolidados heuristicas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/victordesanunes/Documents/artigo-ipo/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7ABF978-4874-ED47-99D8-0E4BC531ACF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{944712DD-07CB-7D42-B7A7-8010615C624F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="84">
   <si>
     <t>dataset</t>
   </si>
@@ -89,13 +89,196 @@
   </si>
   <si>
     <t>bipop</t>
+  </si>
+  <si>
+    <t>Restricted license - for non-production use only - expires 2022-01-13</t>
+  </si>
+  <si>
+    <t>Changed value of parameter NonConvex to 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Prev: -1  Min: -1  Max: 2  Default: -1</t>
+  </si>
+  <si>
+    <t>Gurobi Optimizer version 9.1.2 build v9.1.2rc0 (mac64)</t>
+  </si>
+  <si>
+    <t>Thread count: 2 physical cores, 4 logical processors, using up to 4 threads</t>
+  </si>
+  <si>
+    <t>Optimize a model with 0 rows, 3 columns and 0 nonzeros</t>
+  </si>
+  <si>
+    <t>Model fingerprint: 0x07f362a7</t>
+  </si>
+  <si>
+    <t>Model has 2 quadratic objective terms</t>
+  </si>
+  <si>
+    <t>Coefficient statistics:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Matrix range     [0e+00, 0e+00]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Objective range  [0e+00, 0e+00]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  QObjective range [2e+00, 2e+00]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Bounds range     [0e+00, 0e+00]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  RHS range        [0e+00, 0e+00]</t>
+  </si>
+  <si>
+    <t>Continuous model is non-convex -- solving as a MIP.</t>
+  </si>
+  <si>
+    <t>Found heuristic solution: objective 1.6006911</t>
+  </si>
+  <si>
+    <t>Found heuristic solution: objective -6.53809e+18</t>
+  </si>
+  <si>
+    <t>Presolve time: 0.00s</t>
+  </si>
+  <si>
+    <t>Presolved: 5 rows, 7 columns, 11 nonzeros</t>
+  </si>
+  <si>
+    <t>Presolved model has 2 bilinear constraint(s)</t>
+  </si>
+  <si>
+    <t>Variable types: 7 continuous, 0 integer (0 binary)</t>
+  </si>
+  <si>
+    <t>Root relaxation: unbounded, 3 iterations, 0.00 seconds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Nodes    |    Current Node    |     Objective Bounds      |     Work</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Expl Unexpl |  Obj  Depth IntInf | Incumbent    BestBd   Gap | It/Node Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     0     0  postponed    0      -6.538e+18          -      -     -    0s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     0     2  postponed    0      -6.538e+18          -      -     -    0s</t>
+  </si>
+  <si>
+    <t>*37043 35308             115    -9.85922e+18          -      -   0.1    1s</t>
+  </si>
+  <si>
+    <t>*37045 35308             116    -1.97184e+19          -      -   0.1    1s</t>
+  </si>
+  <si>
+    <t>*37047 35308             117    -3.94369e+19          -      -   0.1    1s</t>
+  </si>
+  <si>
+    <t>*37049 35308             118    -7.88737e+19          -      -   0.1    1s</t>
+  </si>
+  <si>
+    <t>*37051 35308             119    -1.57747e+20          -      -   0.1    1s</t>
+  </si>
+  <si>
+    <t>*37053 35308             120    -3.15495e+20          -      -   0.1    1s</t>
+  </si>
+  <si>
+    <t>*37055 35308             121    -6.30990e+20          -      -   0.1    1s</t>
+  </si>
+  <si>
+    <t>*37057 35308             122    -1.26198e+21          -      -   0.1    1s</t>
+  </si>
+  <si>
+    <t>*37059 35308             123    -2.52396e+21          -      -   0.1    1s</t>
+  </si>
+  <si>
+    <t>*37061 35308             124    -5.04792e+21          -      -   0.1    1s</t>
+  </si>
+  <si>
+    <t>*37063 35308             125    -1.00958e+22          -      -   0.1    1s</t>
+  </si>
+  <si>
+    <t>*37065 35308             126    -2.01917e+22          -      -   0.1    1s</t>
+  </si>
+  <si>
+    <t>*37067 35308             127    -4.03833e+22          -      -   0.1    1s</t>
+  </si>
+  <si>
+    <t>*37069 35308             128    -8.07667e+22          -      -   0.1    1s</t>
+  </si>
+  <si>
+    <t>*37071 35308             129    -1.61533e+23          -      -   0.1    1s</t>
+  </si>
+  <si>
+    <t>*37073 35308             130    -3.23067e+23          -      -   0.1    1s</t>
+  </si>
+  <si>
+    <t>*37075 35308             131    -6.46134e+23          -      -   0.1    1s</t>
+  </si>
+  <si>
+    <t>*37077 35308             132    -1.29227e+24          -      -   0.1    1s</t>
+  </si>
+  <si>
+    <t>*37079 35308             133    -2.58453e+24          -      -   0.1    1s</t>
+  </si>
+  <si>
+    <t>*37081 35308             134    -5.16907e+24          -      -   0.1    1s</t>
+  </si>
+  <si>
+    <t>*37083 35308             135    -1.03381e+25          -      -   0.1    1s</t>
+  </si>
+  <si>
+    <t>*37085 35308             136    -2.06763e+25          -      -   0.1    1s</t>
+  </si>
+  <si>
+    <t>*37947 35308             136    -2.06763e+25          -      -   0.1    1s</t>
+  </si>
+  <si>
+    <t>*51236 46107             139    -5.75097e+25          -      -   0.1    1s</t>
+  </si>
+  <si>
+    <t>*51238 46107             140    -1.15019e+26          -      -   0.1    1s</t>
+  </si>
+  <si>
+    <t>*51242 46107             143    -1.43774e+26          -      -   0.1    1s</t>
+  </si>
+  <si>
+    <t>Explored 54152 nodes (8823 simplex iterations) in 1.95 seconds</t>
+  </si>
+  <si>
+    <t>Thread count was 4 (of 4 available processors)</t>
+  </si>
+  <si>
+    <t>Solution count 10: -1.43774e+26 -1.15019e+26 -5.75097e+25 ... -6.46134e+23</t>
+  </si>
+  <si>
+    <t>Model is unbounded</t>
+  </si>
+  <si>
+    <t>Best objective -1.437741852709e+26, best bound -, gap -</t>
+  </si>
+  <si>
+    <t>Ar 2e+06</t>
+  </si>
+  <si>
+    <t>Br 8.79609e+19</t>
+  </si>
+  <si>
+    <t>cr 999976</t>
+  </si>
+  <si>
+    <t>Obj: -1.43774e+26</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,6 +293,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Var(--jp-code-font-family)"/>
     </font>
   </fonts>
   <fills count="2">
@@ -147,11 +335,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -490,13 +679,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F61"/>
+  <dimension ref="A1:F132"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F5"/>
+      <selection activeCell="A63" sqref="A63:A132"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
@@ -506,7 +695,7 @@
     <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -526,7 +715,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -546,7 +735,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -566,7 +755,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -586,7 +775,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -606,7 +795,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -626,7 +815,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -646,7 +835,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -666,7 +855,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -686,7 +875,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -706,7 +895,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -726,7 +915,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -746,7 +935,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -766,7 +955,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -786,7 +975,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -806,7 +995,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -826,7 +1015,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -846,7 +1035,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -866,7 +1055,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -886,7 +1075,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -906,7 +1095,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -926,7 +1115,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -946,7 +1135,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>14</v>
       </c>
@@ -966,7 +1155,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>14</v>
       </c>
@@ -986,7 +1175,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -1006,7 +1195,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>11</v>
       </c>
@@ -1026,7 +1215,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>11</v>
       </c>
@@ -1046,7 +1235,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>11</v>
       </c>
@@ -1066,7 +1255,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>11</v>
       </c>
@@ -1086,7 +1275,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>12</v>
       </c>
@@ -1106,7 +1295,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
         <v>12</v>
       </c>
@@ -1126,7 +1315,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
         <v>12</v>
       </c>
@@ -1146,7 +1335,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
         <v>12</v>
       </c>
@@ -1166,7 +1355,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
         <v>16</v>
       </c>
@@ -1186,7 +1375,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6">
       <c r="A35" t="s">
         <v>16</v>
       </c>
@@ -1206,7 +1395,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
         <v>16</v>
       </c>
@@ -1226,7 +1415,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
         <v>16</v>
       </c>
@@ -1246,7 +1435,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6">
       <c r="A38" t="s">
         <v>8</v>
       </c>
@@ -1266,7 +1455,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6">
       <c r="A39" t="s">
         <v>8</v>
       </c>
@@ -1286,7 +1475,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6">
       <c r="A40" t="s">
         <v>8</v>
       </c>
@@ -1306,7 +1495,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6">
       <c r="A41" t="s">
         <v>8</v>
       </c>
@@ -1326,7 +1515,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6">
       <c r="A42" t="s">
         <v>10</v>
       </c>
@@ -1346,7 +1535,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6">
       <c r="A43" t="s">
         <v>10</v>
       </c>
@@ -1366,7 +1555,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6">
       <c r="A44" t="s">
         <v>10</v>
       </c>
@@ -1386,7 +1575,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6">
       <c r="A45" t="s">
         <v>10</v>
       </c>
@@ -1406,7 +1595,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6">
       <c r="A46" t="s">
         <v>15</v>
       </c>
@@ -1426,7 +1615,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6">
       <c r="A47" t="s">
         <v>15</v>
       </c>
@@ -1446,7 +1635,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6">
       <c r="A48" t="s">
         <v>15</v>
       </c>
@@ -1466,7 +1655,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6">
       <c r="A49" t="s">
         <v>15</v>
       </c>
@@ -1486,7 +1675,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6">
       <c r="A50" t="s">
         <v>19</v>
       </c>
@@ -1506,7 +1695,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6">
       <c r="A51" t="s">
         <v>19</v>
       </c>
@@ -1526,7 +1715,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6">
       <c r="A52" t="s">
         <v>19</v>
       </c>
@@ -1546,7 +1735,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6">
       <c r="A53" t="s">
         <v>19</v>
       </c>
@@ -1566,7 +1755,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6">
       <c r="A54" t="s">
         <v>18</v>
       </c>
@@ -1586,7 +1775,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6">
       <c r="A55" t="s">
         <v>18</v>
       </c>
@@ -1606,7 +1795,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6">
       <c r="A56" t="s">
         <v>18</v>
       </c>
@@ -1626,7 +1815,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6">
       <c r="A57" t="s">
         <v>18</v>
       </c>
@@ -1646,7 +1835,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6">
       <c r="A58" t="s">
         <v>20</v>
       </c>
@@ -1666,7 +1855,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6">
       <c r="A59" t="s">
         <v>20</v>
       </c>
@@ -1686,7 +1875,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6">
       <c r="A60" t="s">
         <v>20</v>
       </c>
@@ -1706,7 +1895,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6">
       <c r="A61" t="s">
         <v>20</v>
       </c>
@@ -1724,6 +1913,316 @@
       </c>
       <c r="F61">
         <v>0.1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1">
+      <c r="A93" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1">
+      <c r="A94" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1">
+      <c r="A95" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1">
+      <c r="A96" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1">
+      <c r="A100" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1">
+      <c r="A101" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1">
+      <c r="A103" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1">
+      <c r="A104" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1">
+      <c r="A105" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1">
+      <c r="A106" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1">
+      <c r="A107" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1">
+      <c r="A108" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1">
+      <c r="A109" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1">
+      <c r="A110" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1">
+      <c r="A111" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1">
+      <c r="A112" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1">
+      <c r="A113" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1">
+      <c r="A114" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1">
+      <c r="A115" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1">
+      <c r="A116" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1">
+      <c r="A117" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1">
+      <c r="A118" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1">
+      <c r="A119" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1">
+      <c r="A120" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1">
+      <c r="A122" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1">
+      <c r="A123" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1">
+      <c r="A125" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1">
+      <c r="A127" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1">
+      <c r="A128" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1">
+      <c r="A129" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1">
+      <c r="A130" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1">
+      <c r="A131" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1">
+      <c r="A132" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>